<commit_message>
encapsulate functionality to reuse these easily
</commit_message>
<xml_diff>
--- a/output/SecventialSortingResults.xlsx
+++ b/output/SecventialSortingResults.xlsx
@@ -92,7 +92,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0">
-        <v>2.8771950000000004</v>
+        <v>3.261756</v>
       </c>
     </row>
     <row r="3">
@@ -100,7 +100,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0">
-        <v>1.067235</v>
+        <v>1.242801</v>
       </c>
     </row>
     <row r="4">
@@ -108,7 +108,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="0">
-        <v>0.015467</v>
+        <v>0.014614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented parallel aproach and code refactoring
</commit_message>
<xml_diff>
--- a/output/SecventialSortingResults.xlsx
+++ b/output/SecventialSortingResults.xlsx
@@ -92,7 +92,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0">
-        <v>3.261756</v>
+        <v>2.9585820000000003</v>
       </c>
     </row>
     <row r="3">
@@ -100,7 +100,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0">
-        <v>1.242801</v>
+        <v>1.08422</v>
       </c>
     </row>
     <row r="4">
@@ -108,7 +108,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="0">
-        <v>0.014614</v>
+        <v>0.015497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented switch context menu
</commit_message>
<xml_diff>
--- a/output/SecventialSortingResults.xlsx
+++ b/output/SecventialSortingResults.xlsx
@@ -92,7 +92,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0">
-        <v>33.7178418</v>
+        <v>29.9872425</v>
       </c>
     </row>
     <row r="3">
@@ -100,7 +100,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0">
-        <v>12.3117326</v>
+        <v>11.1821577</v>
       </c>
     </row>
     <row r="4">
@@ -108,7 +108,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="0">
-        <v>0.016504</v>
+        <v>0.0145067</v>
       </c>
     </row>
   </sheetData>

</xml_diff>